<commit_message>
Resource file toegevoegd en gebruikt in de back-end. Begin gemaakt met het overzetten van de classes en controller naar een web api om via daar de data in een excel te zetten.
</commit_message>
<xml_diff>
--- a/ASP mvc to excel/Students.xlsx
+++ b/ASP mvc to excel/Students.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Id</t>
   </si>
@@ -26,6 +26,15 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Swen</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Hans</t>
   </si>
   <si>
     <t>Frank</t>
@@ -401,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14ac">
-  <dimension ref="J10:M12"/>
+  <dimension ref="J10:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,29 +432,71 @@
     </row>
     <row r="11">
       <c r="J11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K11" t="s">
         <v>4</v>
       </c>
       <c r="L11">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M11">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="J12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K12" t="s">
         <v>5</v>
       </c>
       <c r="L12">
+        <v>19</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="K13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13">
+        <v>25</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L14">
+        <v>21</v>
+      </c>
+      <c r="M14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="K15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15">
         <v>23</v>
       </c>
-      <c r="M12">
+      <c r="M15">
         <v>2</v>
       </c>
     </row>
@@ -464,7 +515,7 @@
   <sheetData>
     <row r="6">
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>

</xml_diff>